<commit_message>
Finished references (that I could find)
</commit_message>
<xml_diff>
--- a/data-raw/ref-tracker.xlsx
+++ b/data-raw/ref-tracker.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/darcy/Dropbox/R/dendro-db/data-raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A5C1618-230D-C741-A184-CAE572C7F601}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B003A47-8661-D84F-8E6D-80BF69607144}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="5900" windowWidth="27640" windowHeight="16940" xr2:uid="{206E3223-ED34-5642-97AD-BB965CCE923D}"/>
+    <workbookView xWindow="60" yWindow="10740" windowWidth="27640" windowHeight="16940" xr2:uid="{206E3223-ED34-5642-97AD-BB965CCE923D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -25,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="75">
   <si>
     <t>Bannister, Dean and Gell 1966</t>
   </si>
@@ -183,16 +186,73 @@
     <t>bibdex</t>
   </si>
   <si>
-    <t>Bannister1966</t>
-  </si>
-  <si>
-    <t>Bannister1968</t>
-  </si>
-  <si>
-    <t>Robinson1974</t>
-  </si>
-  <si>
     <t>Smiley1983</t>
+  </si>
+  <si>
+    <t>Plog2006</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>Bannister1966-NQ</t>
+  </si>
+  <si>
+    <t>Bannister1966-K</t>
+  </si>
+  <si>
+    <t>Robinson1974-B</t>
+  </si>
+  <si>
+    <t>Robinson1975-HI</t>
+  </si>
+  <si>
+    <t>Bannister1969-SW</t>
+  </si>
+  <si>
+    <t>Bannister1967-J</t>
+  </si>
+  <si>
+    <t>Bannister1970-A</t>
+  </si>
+  <si>
+    <t>Robinson1974-V</t>
+  </si>
+  <si>
+    <t>Bannister1968-CD</t>
+  </si>
+  <si>
+    <t>Bannister1966-E</t>
+  </si>
+  <si>
+    <t>Bannister1971-UW</t>
+  </si>
+  <si>
+    <t>Bannister1970-MNSZ</t>
+  </si>
+  <si>
+    <t>uncertain</t>
+  </si>
+  <si>
+    <t>Dean1975-W</t>
+  </si>
+  <si>
+    <t>Errickson1995</t>
+  </si>
+  <si>
+    <t>no - need to separate</t>
+  </si>
+  <si>
+    <t>Honeycutt1994</t>
+  </si>
+  <si>
+    <t>Nickens1975</t>
+  </si>
+  <si>
+    <t>Robinson1971-DB</t>
+  </si>
+  <si>
+    <t>Towner2008</t>
   </si>
 </sst>
 </file>
@@ -553,8 +613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1C9D2A3-BCF1-9344-AD62-757C52C016A6}">
   <dimension ref="A1:C49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,18 +635,24 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>50</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>50</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -597,247 +663,426 @@
         <v>50</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
         <v>50</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="B8" t="s">
         <v>50</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>50</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>47</v>
+      </c>
+      <c r="B12" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>40</v>
+      </c>
+      <c r="B14" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>37</v>
+      </c>
+      <c r="B15" t="s">
+        <v>50</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
+        <v>1</v>
+      </c>
+      <c r="B16" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+      <c r="B17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+        <v>38</v>
+      </c>
+      <c r="B19" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
+        <v>44</v>
+      </c>
+      <c r="B20" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
+        <v>34</v>
+      </c>
+      <c r="B22" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B23" t="s">
+        <v>50</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+      <c r="B26" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
+        <v>41</v>
+      </c>
+      <c r="B29" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
+        <v>3</v>
+      </c>
+      <c r="B30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="B31" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B32" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B33" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>13</v>
+      </c>
+      <c r="B35" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="B38" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" t="s">
+        <v>50</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B40" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>50</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>5</v>
+      </c>
+      <c r="B42" t="s">
+        <v>50</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>18</v>
+      </c>
+      <c r="B43" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>12</v>
+      </c>
+      <c r="B44" t="s">
+        <v>50</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" t="s">
+        <v>50</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
+      <c r="B46" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>6</v>
+      </c>
+      <c r="B47" t="s">
+        <v>50</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B48" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>7</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>74</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:C1" xr:uid="{B00AB9FF-B482-E845-BADD-634698DE88CA}">
+    <sortState ref="A2:C49">
+      <sortCondition ref="A1:A49"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>

</xml_diff>